<commit_message>
working on simulation - there are some issues with timeline
</commit_message>
<xml_diff>
--- a/Implementation/Data/Data.xlsx
+++ b/Implementation/Data/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Indices Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="41">
   <si>
     <t>Time Horizon (t)</t>
   </si>
@@ -371,7 +371,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-CA"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -512,11 +512,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185202304"/>
-        <c:axId val="185202880"/>
+        <c:axId val="159120704"/>
+        <c:axId val="288882688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="185202304"/>
+        <c:axId val="159120704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,12 +526,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185202880"/>
+        <c:crossAx val="288882688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185202880"/>
+        <c:axId val="288882688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -543,7 +543,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185202304"/>
+        <c:crossAx val="159120704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1951,7 +1951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1986,8 +1986,8 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B2">
-        <f>ROUNDUP(A2^'Indices Data'!B2,0)</f>
-        <v>1</v>
+        <f>ROUNDUP(A2^10,0)</f>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -2142,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,7 +2262,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="19">
-        <v>10</v>
+        <v>10.022</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>1</v>
@@ -2271,7 +2271,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="19">
-        <v>0</v>
+        <v>7.016</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>1</v>
@@ -2280,7 +2280,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="19">
-        <v>0</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="J3" s="20">
         <v>0</v>
@@ -2292,7 +2292,7 @@
         <v>3</v>
       </c>
       <c r="M3" s="20">
-        <v>10</v>
+        <v>10.031000000000001</v>
       </c>
       <c r="N3" s="18">
         <v>1</v>
@@ -2330,7 +2330,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="19">
-        <v>0</v>
+        <v>3.5150000000000001</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>1</v>
@@ -2366,7 +2366,7 @@
         <v>3</v>
       </c>
       <c r="R4" s="19">
-        <v>0</v>
+        <v>4.0090000000000003</v>
       </c>
       <c r="T4" s="9" t="s">
         <v>35</v>
@@ -2389,7 +2389,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="19">
-        <v>0</v>
+        <v>1.1719999999999999</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>1</v>
@@ -2425,7 +2425,7 @@
         <v>3</v>
       </c>
       <c r="R5" s="19">
-        <v>0</v>
+        <v>2.5270000000000001</v>
       </c>
       <c r="T5" s="15" t="s">
         <v>36</v>
@@ -2448,7 +2448,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="19">
-        <v>0</v>
+        <v>7.8E-2</v>
       </c>
       <c r="G6" s="18" t="s">
         <v>1</v>
@@ -2484,7 +2484,7 @@
         <v>3</v>
       </c>
       <c r="R6" s="19">
-        <v>0</v>
+        <v>0.91400000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -2504,7 +2504,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="19">
-        <v>0</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>1</v>
@@ -2540,7 +2540,7 @@
         <v>3</v>
       </c>
       <c r="R7" s="19">
-        <v>0</v>
+        <v>7.0999999999999994E-2</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -2596,7 +2596,7 @@
         <v>3</v>
       </c>
       <c r="R8" s="19">
-        <v>0</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -2824,33 +2824,15 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="19">
-        <v>1</v>
-      </c>
-      <c r="C13" s="19">
-        <v>10</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="21">
-        <v>1</v>
-      </c>
-      <c r="F13" s="19">
-        <v>0</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="19">
-        <v>1</v>
-      </c>
-      <c r="I13" s="19">
-        <v>0</v>
-      </c>
+      <c r="A13" s="23"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
       <c r="J13" s="20">
         <v>10</v>
       </c>
@@ -2880,33 +2862,15 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="19">
-        <v>2</v>
-      </c>
-      <c r="C14" s="19">
-        <v>10</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="21">
-        <v>2</v>
-      </c>
-      <c r="F14" s="19">
-        <v>0</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" s="19">
-        <v>2</v>
-      </c>
-      <c r="I14" s="19">
-        <v>0</v>
-      </c>
+      <c r="A14" s="23"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
       <c r="L14" s="22"/>
@@ -2928,33 +2892,15 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="19">
-        <v>3</v>
-      </c>
-      <c r="C15" s="19">
-        <v>10</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="21">
-        <v>3</v>
-      </c>
-      <c r="F15" s="19">
-        <v>0</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15" s="19">
-        <v>3</v>
-      </c>
-      <c r="I15" s="19">
-        <v>0</v>
-      </c>
+      <c r="A15" s="23"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
       <c r="J15" s="22"/>
       <c r="K15" s="22"/>
       <c r="L15" s="22"/>
@@ -2972,37 +2918,19 @@
         <v>3</v>
       </c>
       <c r="R15" s="19">
-        <v>0</v>
+        <v>2.528</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="19">
-        <v>4</v>
-      </c>
-      <c r="C16" s="19">
-        <v>10</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="21">
-        <v>4</v>
-      </c>
-      <c r="F16" s="19">
-        <v>0</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H16" s="19">
-        <v>4</v>
-      </c>
-      <c r="I16" s="19">
-        <v>0</v>
-      </c>
+      <c r="A16" s="23"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
       <c r="L16" s="22"/>
@@ -3020,37 +2948,19 @@
         <v>3</v>
       </c>
       <c r="R16" s="19">
-        <v>0</v>
+        <v>0.91400000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="19">
-        <v>5</v>
-      </c>
-      <c r="C17" s="19">
-        <v>10</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="21">
-        <v>5</v>
-      </c>
-      <c r="F17" s="19">
-        <v>0</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="19">
-        <v>5</v>
-      </c>
-      <c r="I17" s="19">
-        <v>0</v>
-      </c>
+      <c r="A17" s="23"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
       <c r="L17" s="22"/>
@@ -3068,37 +2978,19 @@
         <v>3</v>
       </c>
       <c r="R17" s="19">
-        <v>0</v>
+        <v>0.24199999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="19">
-        <v>6</v>
-      </c>
-      <c r="C18" s="19">
-        <v>10</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="21">
-        <v>6</v>
-      </c>
-      <c r="F18" s="19">
-        <v>0</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="19">
-        <v>6</v>
-      </c>
-      <c r="I18" s="19">
-        <v>0</v>
-      </c>
+      <c r="A18" s="23"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
       <c r="L18" s="22"/>
@@ -3116,37 +3008,19 @@
         <v>3</v>
       </c>
       <c r="R18" s="19">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="19">
-        <v>7</v>
-      </c>
-      <c r="C19" s="19">
-        <v>10</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="21">
-        <v>7</v>
-      </c>
-      <c r="F19" s="19">
-        <v>0</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19" s="19">
-        <v>7</v>
-      </c>
-      <c r="I19" s="19">
-        <v>0</v>
-      </c>
+      <c r="A19" s="23"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
       <c r="J19" s="22"/>
       <c r="K19" s="22"/>
       <c r="L19" s="22"/>
@@ -3164,37 +3038,19 @@
         <v>3</v>
       </c>
       <c r="R19" s="19">
-        <v>0</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="19">
-        <v>8</v>
-      </c>
-      <c r="C20" s="19">
-        <v>10</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="21">
-        <v>8</v>
-      </c>
-      <c r="F20" s="19">
-        <v>0</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H20" s="19">
-        <v>8</v>
-      </c>
-      <c r="I20" s="19">
-        <v>0</v>
-      </c>
+      <c r="A20" s="23"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
       <c r="J20" s="22"/>
       <c r="K20" s="22"/>
       <c r="L20" s="22"/>
@@ -3216,33 +3072,15 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="19">
-        <v>9</v>
-      </c>
-      <c r="C21" s="19">
-        <v>10</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="21">
-        <v>9</v>
-      </c>
-      <c r="F21" s="19">
-        <v>0</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H21" s="19">
-        <v>9</v>
-      </c>
-      <c r="I21" s="19">
-        <v>0</v>
-      </c>
+      <c r="A21" s="23"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
       <c r="J21" s="22"/>
       <c r="K21" s="22"/>
       <c r="L21" s="22"/>
@@ -3264,33 +3102,15 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="19">
-        <v>10</v>
-      </c>
-      <c r="C22" s="19">
-        <v>10</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="21">
-        <v>10</v>
-      </c>
-      <c r="F22" s="19">
-        <v>0</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H22" s="19">
-        <v>10</v>
-      </c>
-      <c r="I22" s="19">
-        <v>0</v>
-      </c>
+      <c r="A22" s="23"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
@@ -3428,7 +3248,7 @@
         <v>3</v>
       </c>
       <c r="R26" s="19">
-        <v>0</v>
+        <v>0.91400000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -3458,7 +3278,7 @@
         <v>3</v>
       </c>
       <c r="R27" s="19">
-        <v>0</v>
+        <v>0.24099999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -3488,7 +3308,7 @@
         <v>3</v>
       </c>
       <c r="R28" s="19">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -3518,7 +3338,7 @@
         <v>3</v>
       </c>
       <c r="R29" s="19">
-        <v>0</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -3758,7 +3578,7 @@
         <v>3</v>
       </c>
       <c r="R37" s="19">
-        <v>0</v>
+        <v>0.24099999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3788,7 +3608,7 @@
         <v>3</v>
       </c>
       <c r="R38" s="19">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -3818,7 +3638,7 @@
         <v>3</v>
       </c>
       <c r="R39" s="19">
-        <v>0</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -4088,7 +3908,7 @@
         <v>3</v>
       </c>
       <c r="R48" s="19">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
@@ -4118,7 +3938,7 @@
         <v>3</v>
       </c>
       <c r="R49" s="19">
-        <v>0</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
@@ -4327,7 +4147,7 @@
         <v>3</v>
       </c>
       <c r="R59" s="19">
-        <v>0</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
sensitivity analysis & looking for bugs
</commit_message>
<xml_diff>
--- a/Implementation/Data/Data.xlsx
+++ b/Implementation/Data/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Indices Data" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,12 @@
     <sheet name="Expected State Values" sheetId="7" r:id="rId7"/>
     <sheet name="Generate Expected State Values" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="40">
   <si>
     <t>Time Horizon (t)</t>
   </si>
@@ -65,9 +65,6 @@
   <si>
     <t>Deviation (uniform)
 min/max (both inclusive)</t>
-  </si>
-  <si>
-    <t>-10,10</t>
   </si>
   <si>
     <t>CPU</t>
@@ -145,6 +142,12 @@
   </si>
   <si>
     <t>UV</t>
+  </si>
+  <si>
+    <t>-0,0</t>
+  </si>
+  <si>
+    <t>MAYBE THERE ARE BUGS/MODEL ISSUES WITH ^ VALUE</t>
   </si>
 </sst>
 </file>
@@ -354,7 +357,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-CA"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -449,37 +452,37 @@
                   <c:v>1.1000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.21</c:v>
+                  <c:v>1.2100000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.331</c:v>
+                  <c:v>1.3310000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4641</c:v>
+                  <c:v>1.4641000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.610510000000001</c:v>
+                  <c:v>1.6105100000000006</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7715610000000011</c:v>
+                  <c:v>1.7715610000000008</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.948717100000001</c:v>
+                  <c:v>1.9487171000000012</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2.1435888100000011</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.357947691000001</c:v>
+                  <c:v>2.3579476910000015</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2.5937424601000019</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.853116706110002</c:v>
+                  <c:v>2.8531167061100025</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.1384283767210031</c:v>
+                  <c:v>3.1384283767210026</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>3.4522712143931029</c:v>
@@ -500,11 +503,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="207878912"/>
-        <c:axId val="207879488"/>
+        <c:axId val="100670784"/>
+        <c:axId val="218406912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="207878912"/>
+        <c:axId val="100670784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -514,12 +517,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="207879488"/>
+        <c:crossAx val="218406912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="207879488"/>
+        <c:axId val="218406912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -531,7 +534,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="207878912"/>
+        <c:crossAx val="100670784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1036,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,14 +1076,16 @@
         <v>30</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
@@ -1116,16 +1121,16 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1258,7 +1263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1271,13 +1276,13 @@
   <sheetData>
     <row r="1" spans="1:8" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1288,7 +1293,7 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>14.95</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1363,19 +1368,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1920,7 +1925,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,19 +1939,22 @@
   <sheetData>
     <row r="1" spans="1:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="21" t="s">
         <v>25</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>26</v>
       </c>
       <c r="H1" s="22"/>
     </row>
@@ -1955,18 +1963,22 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="C2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D2">
         <v>100</v>
       </c>
-      <c r="D2">
-        <v>0.99</v>
+      <c r="E2">
+        <v>0.95</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
+        <f t="shared" ref="H2:H16" si="0">$A$2^G2</f>
         <v>1</v>
       </c>
     </row>
@@ -1975,29 +1987,26 @@
         <v>1</v>
       </c>
       <c r="H3">
+        <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
-        <v>27</v>
-      </c>
+    <row r="4" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4">
-        <v>1.21</v>
+        <f t="shared" si="0"/>
+        <v>1.2100000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>1.1000000000000001</v>
-      </c>
       <c r="G5">
         <v>3</v>
       </c>
       <c r="H5">
-        <v>1.331</v>
+        <f t="shared" si="0"/>
+        <v>1.3310000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2005,7 +2014,8 @@
         <v>4</v>
       </c>
       <c r="H6">
-        <v>1.4641</v>
+        <f t="shared" si="0"/>
+        <v>1.4641000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2013,7 +2023,8 @@
         <v>5</v>
       </c>
       <c r="H7">
-        <v>1.610510000000001</v>
+        <f t="shared" si="0"/>
+        <v>1.6105100000000006</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2021,7 +2032,8 @@
         <v>6</v>
       </c>
       <c r="H8">
-        <v>1.7715610000000011</v>
+        <f t="shared" si="0"/>
+        <v>1.7715610000000008</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2029,7 +2041,8 @@
         <v>7</v>
       </c>
       <c r="H9">
-        <v>1.948717100000001</v>
+        <f t="shared" si="0"/>
+        <v>1.9487171000000012</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2037,6 +2050,7 @@
         <v>8</v>
       </c>
       <c r="H10">
+        <f t="shared" si="0"/>
         <v>2.1435888100000011</v>
       </c>
     </row>
@@ -2045,7 +2059,8 @@
         <v>9</v>
       </c>
       <c r="H11">
-        <v>2.357947691000001</v>
+        <f t="shared" si="0"/>
+        <v>2.3579476910000015</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2053,6 +2068,7 @@
         <v>10</v>
       </c>
       <c r="H12">
+        <f t="shared" si="0"/>
         <v>2.5937424601000019</v>
       </c>
     </row>
@@ -2061,7 +2077,8 @@
         <v>11</v>
       </c>
       <c r="H13">
-        <v>2.853116706110002</v>
+        <f t="shared" si="0"/>
+        <v>2.8531167061100025</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2069,7 +2086,8 @@
         <v>12</v>
       </c>
       <c r="H14">
-        <v>3.1384283767210031</v>
+        <f t="shared" si="0"/>
+        <v>3.1384283767210026</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2077,6 +2095,7 @@
         <v>13</v>
       </c>
       <c r="H15">
+        <f t="shared" si="0"/>
         <v>3.4522712143931029</v>
       </c>
     </row>
@@ -2085,6 +2104,7 @@
         <v>14</v>
       </c>
       <c r="H16">
+        <f t="shared" si="0"/>
         <v>3.7974983358324139</v>
       </c>
     </row>
@@ -2103,7 +2123,7 @@
   <dimension ref="A1:Q442"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC6" sqref="AC6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2127,23 +2147,23 @@
   <sheetData>
     <row r="1" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
       <c r="D1" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="22"/>
       <c r="F1" s="22"/>
       <c r="G1" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
       <c r="J1" s="20"/>
       <c r="K1" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
@@ -2152,49 +2172,49 @@
     </row>
     <row r="2" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="H2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="L2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -2205,7 +2225,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="14">
-        <v>31.132000000000001</v>
+        <v>30</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>6</v>
@@ -2214,7 +2234,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="15">
-        <v>27.887</v>
+        <v>30</v>
       </c>
       <c r="G3" s="13">
         <v>0</v>
@@ -2226,7 +2246,7 @@
         <v>8</v>
       </c>
       <c r="J3" s="13">
-        <v>30.071000000000002</v>
+        <v>15</v>
       </c>
       <c r="K3" s="15">
         <v>1</v>
@@ -2241,7 +2261,7 @@
         <v>8</v>
       </c>
       <c r="O3" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -2261,7 +2281,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="15">
-        <v>24.838000000000001</v>
+        <v>30</v>
       </c>
       <c r="G4" s="13">
         <v>1</v>
@@ -2273,7 +2293,7 @@
         <v>8</v>
       </c>
       <c r="J4" s="13">
-        <v>4.92</v>
+        <v>15</v>
       </c>
       <c r="K4" s="15">
         <v>1</v>
@@ -2288,7 +2308,7 @@
         <v>8</v>
       </c>
       <c r="O4" s="15">
-        <v>2.1800000000000002</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -2308,7 +2328,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="15">
-        <v>22.725000000000001</v>
+        <v>30</v>
       </c>
       <c r="G5" s="13">
         <v>2</v>
@@ -2320,7 +2340,7 @@
         <v>8</v>
       </c>
       <c r="J5" s="13">
-        <v>4.383</v>
+        <v>15</v>
       </c>
       <c r="K5" s="15">
         <v>1</v>
@@ -2335,7 +2355,7 @@
         <v>8</v>
       </c>
       <c r="O5" s="15">
-        <v>0.93799999999999994</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2355,7 +2375,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="15">
-        <v>20.539000000000001</v>
+        <v>30</v>
       </c>
       <c r="G6" s="13">
         <v>3</v>
@@ -2367,7 +2387,7 @@
         <v>8</v>
       </c>
       <c r="J6" s="13">
-        <v>3.8239999999999998</v>
+        <v>15</v>
       </c>
       <c r="K6" s="15">
         <v>1</v>
@@ -2382,7 +2402,7 @@
         <v>8</v>
       </c>
       <c r="O6" s="15">
-        <v>1.056</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2402,7 +2422,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="15">
-        <v>17.748999999999999</v>
+        <v>30</v>
       </c>
       <c r="G7" s="13">
         <v>4</v>
@@ -2414,7 +2434,7 @@
         <v>8</v>
       </c>
       <c r="J7" s="13">
-        <v>3.367</v>
+        <v>15</v>
       </c>
       <c r="K7" s="15">
         <v>1</v>
@@ -2429,7 +2449,7 @@
         <v>8</v>
       </c>
       <c r="O7" s="15">
-        <v>1.3460000000000001</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2449,7 +2469,7 @@
         <v>6</v>
       </c>
       <c r="F8" s="15">
-        <v>15.79</v>
+        <v>30</v>
       </c>
       <c r="G8" s="13">
         <v>5</v>
@@ -2461,7 +2481,7 @@
         <v>8</v>
       </c>
       <c r="J8" s="13">
-        <v>2.9470000000000001</v>
+        <v>15</v>
       </c>
       <c r="K8" s="15">
         <v>1</v>
@@ -2476,7 +2496,7 @@
         <v>8</v>
       </c>
       <c r="O8" s="15">
-        <v>0.90200000000000002</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2496,7 +2516,7 @@
         <v>7</v>
       </c>
       <c r="F9" s="15">
-        <v>14.273</v>
+        <v>30</v>
       </c>
       <c r="G9" s="13">
         <v>6</v>
@@ -2508,7 +2528,7 @@
         <v>8</v>
       </c>
       <c r="J9" s="13">
-        <v>2.101</v>
+        <v>15</v>
       </c>
       <c r="K9" s="15">
         <v>1</v>
@@ -2523,7 +2543,7 @@
         <v>8</v>
       </c>
       <c r="O9" s="15">
-        <v>0.68899999999999995</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -2543,7 +2563,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="15">
-        <v>13.303000000000001</v>
+        <v>30</v>
       </c>
       <c r="G10" s="13">
         <v>7</v>
@@ -2555,7 +2575,7 @@
         <v>8</v>
       </c>
       <c r="J10" s="13">
-        <v>1.3220000000000001</v>
+        <v>15</v>
       </c>
       <c r="K10" s="15">
         <v>1</v>
@@ -2570,7 +2590,7 @@
         <v>8</v>
       </c>
       <c r="O10" s="15">
-        <v>0.499</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2590,7 +2610,7 @@
         <v>9</v>
       </c>
       <c r="F11" s="15">
-        <v>11.714</v>
+        <v>30</v>
       </c>
       <c r="G11" s="13">
         <v>8</v>
@@ -2602,7 +2622,7 @@
         <v>8</v>
       </c>
       <c r="J11" s="13">
-        <v>0.80700000000000005</v>
+        <v>15</v>
       </c>
       <c r="K11" s="15">
         <v>1</v>
@@ -2617,7 +2637,7 @@
         <v>8</v>
       </c>
       <c r="O11" s="15">
-        <v>0.75</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -2637,7 +2657,7 @@
         <v>10</v>
       </c>
       <c r="F12" s="15">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G12" s="13">
         <v>9</v>
@@ -2649,7 +2669,7 @@
         <v>8</v>
       </c>
       <c r="J12" s="13">
-        <v>0.29499999999999998</v>
+        <v>15</v>
       </c>
       <c r="K12" s="15">
         <v>1</v>
@@ -2664,7 +2684,7 @@
         <v>8</v>
       </c>
       <c r="O12" s="15">
-        <v>0.64700000000000002</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2684,7 +2704,7 @@
         <v>8</v>
       </c>
       <c r="J13" s="13">
-        <v>0.82899999999999996</v>
+        <v>15</v>
       </c>
       <c r="K13" s="15">
         <v>1</v>
@@ -2699,7 +2719,7 @@
         <v>8</v>
       </c>
       <c r="O13" s="15">
-        <v>4.9370000000000003</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2726,7 +2746,7 @@
         <v>8</v>
       </c>
       <c r="O14" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2753,7 +2773,7 @@
         <v>8</v>
       </c>
       <c r="O15" s="15">
-        <v>1.0269999999999999</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2780,7 +2800,7 @@
         <v>8</v>
       </c>
       <c r="O16" s="15">
-        <v>1.1040000000000001</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -2807,7 +2827,7 @@
         <v>8</v>
       </c>
       <c r="O17" s="15">
-        <v>1.39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -2834,7 +2854,7 @@
         <v>8</v>
       </c>
       <c r="O18" s="15">
-        <v>0.96799999999999997</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -2861,7 +2881,7 @@
         <v>8</v>
       </c>
       <c r="O19" s="15">
-        <v>0.72</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -2888,7 +2908,7 @@
         <v>8</v>
       </c>
       <c r="O20" s="15">
-        <v>0.45500000000000002</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -2915,7 +2935,7 @@
         <v>8</v>
       </c>
       <c r="O21" s="15">
-        <v>0.75600000000000001</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -2942,7 +2962,7 @@
         <v>8</v>
       </c>
       <c r="O22" s="15">
-        <v>0.67500000000000004</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -2963,7 +2983,7 @@
         <v>8</v>
       </c>
       <c r="O23" s="15">
-        <v>0.54300000000000004</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -2984,7 +3004,7 @@
         <v>8</v>
       </c>
       <c r="O24" s="15">
-        <v>4.782</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -3005,7 +3025,7 @@
         <v>8</v>
       </c>
       <c r="O25" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -3026,7 +3046,7 @@
         <v>8</v>
       </c>
       <c r="O26" s="15">
-        <v>1.0760000000000001</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -3047,7 +3067,7 @@
         <v>8</v>
       </c>
       <c r="O27" s="15">
-        <v>1.3779999999999999</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -3068,7 +3088,7 @@
         <v>8</v>
       </c>
       <c r="O28" s="15">
-        <v>0.96899999999999997</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -3089,7 +3109,7 @@
         <v>8</v>
       </c>
       <c r="O29" s="15">
-        <v>0.72</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -3110,7 +3130,7 @@
         <v>8</v>
       </c>
       <c r="O30" s="15">
-        <v>0.45400000000000001</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -3131,7 +3151,7 @@
         <v>8</v>
       </c>
       <c r="O31" s="15">
-        <v>0.75700000000000001</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -3152,7 +3172,7 @@
         <v>8</v>
       </c>
       <c r="O32" s="15">
-        <v>0.67</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="7:15" x14ac:dyDescent="0.25">
@@ -3173,7 +3193,7 @@
         <v>8</v>
       </c>
       <c r="O33" s="15">
-        <v>0.54400000000000004</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="7:15" x14ac:dyDescent="0.25">
@@ -3194,7 +3214,7 @@
         <v>8</v>
       </c>
       <c r="O34" s="15">
-        <v>0.55500000000000005</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="7:15" x14ac:dyDescent="0.25">
@@ -3215,7 +3235,7 @@
         <v>8</v>
       </c>
       <c r="O35" s="15">
-        <v>4.2389999999999999</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="7:15" x14ac:dyDescent="0.25">
@@ -3236,7 +3256,7 @@
         <v>8</v>
       </c>
       <c r="O36" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="7:15" x14ac:dyDescent="0.25">
@@ -3257,7 +3277,7 @@
         <v>8</v>
       </c>
       <c r="O37" s="15">
-        <v>1.3660000000000001</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="7:15" x14ac:dyDescent="0.25">
@@ -3278,7 +3298,7 @@
         <v>8</v>
       </c>
       <c r="O38" s="15">
-        <v>0.96199999999999997</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="7:15" x14ac:dyDescent="0.25">
@@ -3299,7 +3319,7 @@
         <v>8</v>
       </c>
       <c r="O39" s="15">
-        <v>0.71299999999999997</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="7:15" x14ac:dyDescent="0.25">
@@ -3320,7 +3340,7 @@
         <v>8</v>
       </c>
       <c r="O40" s="15">
-        <v>0.45400000000000001</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="7:15" x14ac:dyDescent="0.25">
@@ -3341,7 +3361,7 @@
         <v>8</v>
       </c>
       <c r="O41" s="15">
-        <v>0.75600000000000001</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="7:15" x14ac:dyDescent="0.25">
@@ -3362,7 +3382,7 @@
         <v>8</v>
       </c>
       <c r="O42" s="15">
-        <v>0.66500000000000004</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="7:15" x14ac:dyDescent="0.25">
@@ -3383,7 +3403,7 @@
         <v>8</v>
       </c>
       <c r="O43" s="15">
-        <v>0.54400000000000004</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="7:15" x14ac:dyDescent="0.25">
@@ -3404,7 +3424,7 @@
         <v>8</v>
       </c>
       <c r="O44" s="15">
-        <v>0.55800000000000005</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="7:15" x14ac:dyDescent="0.25">
@@ -3425,7 +3445,7 @@
         <v>8</v>
       </c>
       <c r="O45" s="15">
-        <v>0.45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="7:15" x14ac:dyDescent="0.25">
@@ -3446,7 +3466,7 @@
         <v>8</v>
       </c>
       <c r="O46" s="15">
-        <v>3.8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="7:15" x14ac:dyDescent="0.25">
@@ -3463,7 +3483,7 @@
         <v>8</v>
       </c>
       <c r="O47" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="7:15" x14ac:dyDescent="0.25">
@@ -3480,7 +3500,7 @@
         <v>8</v>
       </c>
       <c r="O48" s="15">
-        <v>0.95799999999999996</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="11:15" x14ac:dyDescent="0.25">
@@ -3497,7 +3517,7 @@
         <v>8</v>
       </c>
       <c r="O49" s="15">
-        <v>0.70799999999999996</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="11:15" x14ac:dyDescent="0.25">
@@ -3514,7 +3534,7 @@
         <v>8</v>
       </c>
       <c r="O50" s="15">
-        <v>0.439</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="11:15" x14ac:dyDescent="0.25">
@@ -3531,7 +3551,7 @@
         <v>8</v>
       </c>
       <c r="O51" s="15">
-        <v>0.746</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="11:15" x14ac:dyDescent="0.25">
@@ -3548,7 +3568,7 @@
         <v>8</v>
       </c>
       <c r="O52" s="15">
-        <v>0.65700000000000003</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="11:15" x14ac:dyDescent="0.25">
@@ -3565,7 +3585,7 @@
         <v>8</v>
       </c>
       <c r="O53" s="15">
-        <v>0.54600000000000004</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="11:15" x14ac:dyDescent="0.25">
@@ -3582,7 +3602,7 @@
         <v>8</v>
       </c>
       <c r="O54" s="15">
-        <v>0.55900000000000005</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="11:15" x14ac:dyDescent="0.25">
@@ -3599,7 +3619,7 @@
         <v>8</v>
       </c>
       <c r="O55" s="15">
-        <v>0.45500000000000002</v>
+        <v>15</v>
       </c>
     </row>
     <row r="56" spans="11:15" x14ac:dyDescent="0.25">
@@ -3616,7 +3636,7 @@
         <v>8</v>
       </c>
       <c r="O56" s="15">
-        <v>0.48499999999999999</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="11:15" x14ac:dyDescent="0.25">
@@ -3633,7 +3653,7 @@
         <v>8</v>
       </c>
       <c r="O57" s="15">
-        <v>3.3220000000000001</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="11:15" x14ac:dyDescent="0.25">
@@ -3650,7 +3670,7 @@
         <v>8</v>
       </c>
       <c r="O58" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="11:15" x14ac:dyDescent="0.25">
@@ -3667,7 +3687,7 @@
         <v>8</v>
       </c>
       <c r="O59" s="15">
-        <v>0.70499999999999996</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="11:15" x14ac:dyDescent="0.25">
@@ -3684,7 +3704,7 @@
         <v>8</v>
       </c>
       <c r="O60" s="15">
-        <v>0.433</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="11:15" x14ac:dyDescent="0.25">
@@ -3701,7 +3721,7 @@
         <v>8</v>
       </c>
       <c r="O61" s="15">
-        <v>0.74099999999999999</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62" spans="11:15" x14ac:dyDescent="0.25">
@@ -3718,7 +3738,7 @@
         <v>8</v>
       </c>
       <c r="O62" s="15">
-        <v>0.64600000000000002</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="11:15" x14ac:dyDescent="0.25">
@@ -3735,7 +3755,7 @@
         <v>8</v>
       </c>
       <c r="O63" s="15">
-        <v>0.54200000000000004</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="11:15" x14ac:dyDescent="0.25">
@@ -3752,7 +3772,7 @@
         <v>8</v>
       </c>
       <c r="O64" s="15">
-        <v>0.55800000000000005</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" spans="11:15" x14ac:dyDescent="0.25">
@@ -3769,7 +3789,7 @@
         <v>8</v>
       </c>
       <c r="O65" s="15">
-        <v>0.46</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="11:15" x14ac:dyDescent="0.25">
@@ -3786,7 +3806,7 @@
         <v>8</v>
       </c>
       <c r="O66" s="15">
-        <v>0.48299999999999998</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="11:15" x14ac:dyDescent="0.25">
@@ -3803,7 +3823,7 @@
         <v>8</v>
       </c>
       <c r="O67" s="15">
-        <v>0.82699999999999996</v>
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="11:15" x14ac:dyDescent="0.25">
@@ -3820,7 +3840,7 @@
         <v>8</v>
       </c>
       <c r="O68" s="15">
-        <v>2.4990000000000001</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="11:15" x14ac:dyDescent="0.25">
@@ -3837,7 +3857,7 @@
         <v>8</v>
       </c>
       <c r="O69" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="11:15" x14ac:dyDescent="0.25">
@@ -3854,7 +3874,7 @@
         <v>8</v>
       </c>
       <c r="O70" s="15">
-        <v>0.43099999999999999</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="11:15" x14ac:dyDescent="0.25">
@@ -3871,7 +3891,7 @@
         <v>8</v>
       </c>
       <c r="O71" s="15">
-        <v>0.73699999999999999</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="11:15" x14ac:dyDescent="0.25">
@@ -3888,7 +3908,7 @@
         <v>8</v>
       </c>
       <c r="O72" s="15">
-        <v>0.63200000000000001</v>
+        <v>15</v>
       </c>
     </row>
     <row r="73" spans="11:15" x14ac:dyDescent="0.25">
@@ -3905,7 +3925,7 @@
         <v>8</v>
       </c>
       <c r="O73" s="15">
-        <v>0.53</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="11:15" x14ac:dyDescent="0.25">
@@ -3922,7 +3942,7 @@
         <v>8</v>
       </c>
       <c r="O74" s="15">
-        <v>0.54400000000000004</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="11:15" x14ac:dyDescent="0.25">
@@ -3939,7 +3959,7 @@
         <v>8</v>
       </c>
       <c r="O75" s="15">
-        <v>0.45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="76" spans="11:15" x14ac:dyDescent="0.25">
@@ -3956,7 +3976,7 @@
         <v>8</v>
       </c>
       <c r="O76" s="15">
-        <v>0.47899999999999998</v>
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="11:15" x14ac:dyDescent="0.25">
@@ -3973,7 +3993,7 @@
         <v>8</v>
       </c>
       <c r="O77" s="15">
-        <v>0.82899999999999996</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78" spans="11:15" x14ac:dyDescent="0.25">
@@ -3990,7 +4010,7 @@
         <v>8</v>
       </c>
       <c r="O78" s="15">
-        <v>0.73399999999999999</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" spans="11:15" x14ac:dyDescent="0.25">
@@ -4007,7 +4027,7 @@
         <v>8</v>
       </c>
       <c r="O79" s="15">
-        <v>1.7709999999999999</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="11:15" x14ac:dyDescent="0.25">
@@ -4024,7 +4044,7 @@
         <v>8</v>
       </c>
       <c r="O80" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="11:15" x14ac:dyDescent="0.25">
@@ -4041,7 +4061,7 @@
         <v>8</v>
       </c>
       <c r="O81" s="15">
-        <v>0.73299999999999998</v>
+        <v>15</v>
       </c>
     </row>
     <row r="82" spans="11:15" x14ac:dyDescent="0.25">
@@ -4058,7 +4078,7 @@
         <v>8</v>
       </c>
       <c r="O82" s="15">
-        <v>0.62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83" spans="11:15" x14ac:dyDescent="0.25">
@@ -4075,7 +4095,7 @@
         <v>8</v>
       </c>
       <c r="O83" s="15">
-        <v>0.52100000000000002</v>
+        <v>15</v>
       </c>
     </row>
     <row r="84" spans="11:15" x14ac:dyDescent="0.25">
@@ -4092,7 +4112,7 @@
         <v>8</v>
       </c>
       <c r="O84" s="15">
-        <v>0.53100000000000003</v>
+        <v>15</v>
       </c>
     </row>
     <row r="85" spans="11:15" x14ac:dyDescent="0.25">
@@ -4109,7 +4129,7 @@
         <v>8</v>
       </c>
       <c r="O85" s="15">
-        <v>0.44400000000000001</v>
+        <v>15</v>
       </c>
     </row>
     <row r="86" spans="11:15" x14ac:dyDescent="0.25">
@@ -4126,7 +4146,7 @@
         <v>8</v>
       </c>
       <c r="O86" s="15">
-        <v>0.46600000000000003</v>
+        <v>15</v>
       </c>
     </row>
     <row r="87" spans="11:15" x14ac:dyDescent="0.25">
@@ -4143,7 +4163,7 @@
         <v>8</v>
       </c>
       <c r="O87" s="15">
-        <v>0.82899999999999996</v>
+        <v>15</v>
       </c>
     </row>
     <row r="88" spans="11:15" x14ac:dyDescent="0.25">
@@ -4160,7 +4180,7 @@
         <v>8</v>
       </c>
       <c r="O88" s="15">
-        <v>0.73599999999999999</v>
+        <v>15</v>
       </c>
     </row>
     <row r="89" spans="11:15" x14ac:dyDescent="0.25">
@@ -4177,7 +4197,7 @@
         <v>8</v>
       </c>
       <c r="O89" s="15">
-        <v>0.496</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="11:15" x14ac:dyDescent="0.25">
@@ -4194,7 +4214,7 @@
         <v>8</v>
       </c>
       <c r="O90" s="15">
-        <v>1.2749999999999999</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91" spans="11:15" x14ac:dyDescent="0.25">
@@ -4211,7 +4231,7 @@
         <v>8</v>
       </c>
       <c r="O91" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="92" spans="11:15" x14ac:dyDescent="0.25">
@@ -4228,7 +4248,7 @@
         <v>8</v>
       </c>
       <c r="O92" s="15">
-        <v>0.59899999999999998</v>
+        <v>15</v>
       </c>
     </row>
     <row r="93" spans="11:15" x14ac:dyDescent="0.25">
@@ -4245,7 +4265,7 @@
         <v>8</v>
       </c>
       <c r="O93" s="15">
-        <v>0.51800000000000002</v>
+        <v>15</v>
       </c>
     </row>
     <row r="94" spans="11:15" x14ac:dyDescent="0.25">
@@ -4262,7 +4282,7 @@
         <v>8</v>
       </c>
       <c r="O94" s="15">
-        <v>0.53600000000000003</v>
+        <v>15</v>
       </c>
     </row>
     <row r="95" spans="11:15" x14ac:dyDescent="0.25">
@@ -4279,7 +4299,7 @@
         <v>8</v>
       </c>
       <c r="O95" s="15">
-        <v>0.434</v>
+        <v>15</v>
       </c>
     </row>
     <row r="96" spans="11:15" x14ac:dyDescent="0.25">
@@ -4296,7 +4316,7 @@
         <v>8</v>
       </c>
       <c r="O96" s="15">
-        <v>0.45300000000000001</v>
+        <v>15</v>
       </c>
     </row>
     <row r="97" spans="11:15" x14ac:dyDescent="0.25">
@@ -4313,7 +4333,7 @@
         <v>8</v>
       </c>
       <c r="O97" s="15">
-        <v>0.82299999999999995</v>
+        <v>15</v>
       </c>
     </row>
     <row r="98" spans="11:15" x14ac:dyDescent="0.25">
@@ -4330,7 +4350,7 @@
         <v>8</v>
       </c>
       <c r="O98" s="15">
-        <v>0.73099999999999998</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99" spans="11:15" x14ac:dyDescent="0.25">
@@ -4347,7 +4367,7 @@
         <v>8</v>
       </c>
       <c r="O99" s="15">
-        <v>0.49199999999999999</v>
+        <v>15</v>
       </c>
     </row>
     <row r="100" spans="11:15" x14ac:dyDescent="0.25">
@@ -4364,7 +4384,7 @@
         <v>8</v>
       </c>
       <c r="O100" s="15">
-        <v>0.54900000000000004</v>
+        <v>15</v>
       </c>
     </row>
     <row r="101" spans="11:15" x14ac:dyDescent="0.25">
@@ -4381,7 +4401,7 @@
         <v>8</v>
       </c>
       <c r="O101" s="15">
-        <v>0.72199999999999998</v>
+        <v>15</v>
       </c>
     </row>
     <row r="102" spans="11:15" x14ac:dyDescent="0.25">
@@ -4398,7 +4418,7 @@
         <v>8</v>
       </c>
       <c r="O102" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="103" spans="11:15" x14ac:dyDescent="0.25">
@@ -4415,7 +4435,7 @@
         <v>8</v>
       </c>
       <c r="O103" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="104" spans="11:15" x14ac:dyDescent="0.25">
@@ -4432,7 +4452,7 @@
         <v>8</v>
       </c>
       <c r="O104" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="105" spans="11:15" x14ac:dyDescent="0.25">
@@ -4449,7 +4469,7 @@
         <v>8</v>
       </c>
       <c r="O105" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="11:15" x14ac:dyDescent="0.25">
@@ -4466,7 +4486,7 @@
         <v>8</v>
       </c>
       <c r="O106" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107" spans="11:15" x14ac:dyDescent="0.25">
@@ -4483,7 +4503,7 @@
         <v>8</v>
       </c>
       <c r="O107" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="108" spans="11:15" x14ac:dyDescent="0.25">
@@ -4500,7 +4520,7 @@
         <v>8</v>
       </c>
       <c r="O108" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="109" spans="11:15" x14ac:dyDescent="0.25">
@@ -4517,7 +4537,7 @@
         <v>8</v>
       </c>
       <c r="O109" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="110" spans="11:15" x14ac:dyDescent="0.25">
@@ -4534,7 +4554,7 @@
         <v>8</v>
       </c>
       <c r="O110" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="111" spans="11:15" x14ac:dyDescent="0.25">
@@ -4551,7 +4571,7 @@
         <v>8</v>
       </c>
       <c r="O111" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="112" spans="11:15" x14ac:dyDescent="0.25">
@@ -4568,7 +4588,7 @@
         <v>8</v>
       </c>
       <c r="O112" s="15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="113" spans="11:15" x14ac:dyDescent="0.25">
@@ -6898,7 +6918,7 @@
   <dimension ref="A1:R442"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6924,28 +6944,28 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
       <c r="D1" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="22"/>
       <c r="F1" s="22"/>
       <c r="G1" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
       <c r="J1" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
       <c r="N1" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O1" s="22"/>
       <c r="P1" s="22"/>
@@ -6954,58 +6974,58 @@
     </row>
     <row r="2" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="K2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="O2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finished sensitivity analysis with no deviation
</commit_message>
<xml_diff>
--- a/Implementation/Data/Data.xlsx
+++ b/Implementation/Data/Data.xlsx
@@ -503,11 +503,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="100670784"/>
-        <c:axId val="218406912"/>
+        <c:axId val="86105408"/>
+        <c:axId val="173121536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100670784"/>
+        <c:axId val="86105408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -517,12 +517,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="218406912"/>
+        <c:crossAx val="173121536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218406912"/>
+        <c:axId val="173121536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -534,7 +534,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100670784"/>
+        <c:crossAx val="86105408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1040,7 +1040,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>